<commit_message>
develope to date function
</commit_message>
<xml_diff>
--- a/Data/database/值班人員名列.xlsx
+++ b/Data/database/值班人員名列.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lch/program/新竹榮總/排班/Data/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lch/program/新竹榮總/排班/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B501840-4EB6-5A4F-8DF8-3087216C08ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDB3245-D100-4243-9C9F-E1D806EBA3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2D775E5C-1356-D041-9AA5-9FA63AB1D172}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{2D775E5C-1356-D041-9AA5-9FA63AB1D172}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>名稱</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -555,7 +555,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -635,9 +635,6 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
       <c r="F5" t="s">
         <v>46</v>
       </c>
@@ -649,9 +646,6 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
       <c r="F6" t="s">
         <v>46</v>
       </c>
@@ -663,9 +657,6 @@
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
       <c r="F7" t="s">
         <v>46</v>
       </c>
@@ -680,9 +671,6 @@
       <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
       <c r="F8" t="s">
         <v>46</v>
       </c>
@@ -694,9 +682,6 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
-        <v>46</v>
-      </c>
       <c r="F9" t="s">
         <v>46</v>
       </c>
@@ -711,9 +696,6 @@
       <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
       <c r="F10" t="s">
         <v>46</v>
       </c>
@@ -725,12 +707,6 @@
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" t="s">
-        <v>46</v>
-      </c>
       <c r="G11" t="s">
         <v>46</v>
       </c>
@@ -742,12 +718,6 @@
       <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" t="s">
-        <v>46</v>
-      </c>
       <c r="G12" t="s">
         <v>46</v>
       </c>
@@ -756,12 +726,6 @@
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" t="s">
-        <v>46</v>
-      </c>
       <c r="G13" t="s">
         <v>46</v>
       </c>
@@ -770,12 +734,6 @@
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" t="s">
-        <v>46</v>
-      </c>
       <c r="G14" t="s">
         <v>46</v>
       </c>
@@ -784,12 +742,6 @@
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" t="s">
-        <v>46</v>
-      </c>
       <c r="G15" t="s">
         <v>46</v>
       </c>
@@ -801,86 +753,44 @@
       <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" t="s">
-        <v>46</v>
-      </c>
       <c r="G16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="E18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E19" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E20" t="s">
-        <v>46</v>
-      </c>
-      <c r="G20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E21" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E22" t="s">
-        <v>46</v>
-      </c>
-      <c r="G22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -890,107 +800,56 @@
       <c r="D23" t="s">
         <v>41</v>
       </c>
-      <c r="E23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E24" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E25" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>36</v>
       </c>
-      <c r="E26" t="s">
-        <v>46</v>
-      </c>
-      <c r="G26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E27" t="s">
-        <v>46</v>
-      </c>
-      <c r="G27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="E28" t="s">
-        <v>46</v>
-      </c>
-      <c r="G28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E29" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="G32" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:1">

</xml_diff>